<commit_message>
made progress on inside electronics :tophat:
</commit_message>
<xml_diff>
--- a/cad/rough stuff/rough dimensions calculations.xlsx
+++ b/cad/rough stuff/rough dimensions calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ZEDD-VALORANT-SWORD-thingy\cad\rough stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88258DE1-1D45-4FB7-8BD7-249466B3959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35925AB0-C0DA-4A84-B412-366B1C89F41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>BLADE:</t>
   </si>
@@ -106,6 +106,27 @@
   </si>
   <si>
     <t>17.75 inches</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>2.13mm</t>
+  </si>
+  <si>
+    <t>12mm</t>
+  </si>
+  <si>
+    <t>one led piece</t>
+  </si>
+  <si>
+    <t>6.9mm</t>
+  </si>
+  <si>
+    <t>1.92mm</t>
+  </si>
+  <si>
+    <t>between leds</t>
   </si>
 </sst>
 </file>
@@ -194,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -220,6 +241,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -230,9 +256,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,7 +582,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -715,14 +743,14 @@
       <c r="B7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -785,11 +813,11 @@
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -799,11 +827,11 @@
       <c r="A13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -813,10 +841,10 @@
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -826,16 +854,16 @@
       <c r="B15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -857,6 +885,39 @@
       </c>
       <c r="G16" s="13" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>